<commit_message>
Added new fasta file
</commit_message>
<xml_diff>
--- a/VoucherGenerator/Penghuni RTB New.xlsx
+++ b/VoucherGenerator/Penghuni RTB New.xlsx
@@ -5,17 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Console-Application\VoucherGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA81E2D-EF70-4001-B57A-F289A80389A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2EED1C-26B7-4FAC-BD20-D221F3FA814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023-2024" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1759,7 +1772,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.7109375" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1768,8 +1781,8 @@
     <col min="2" max="2" width="11.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="15" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="14" customWidth="1"/>
-    <col min="5" max="12" width="35.7109375" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="35.7109375" style="4"/>
+    <col min="5" max="15" width="35.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="35.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1839,7 +1852,7 @@
         <v>920210</v>
       </c>
       <c r="D5" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1881,7 +1894,7 @@
         <v>287743</v>
       </c>
       <c r="D8" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2007,7 +2020,7 @@
         <v>121955</v>
       </c>
       <c r="D17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2119,7 +2132,7 @@
         <v>156841</v>
       </c>
       <c r="D25" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2217,7 +2230,7 @@
         <v>169507</v>
       </c>
       <c r="D32" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2273,7 +2286,7 @@
         <v>406947</v>
       </c>
       <c r="D36" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2329,7 +2342,7 @@
         <v>133497</v>
       </c>
       <c r="D40" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2343,7 +2356,7 @@
         <v>552393</v>
       </c>
       <c r="D41" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2413,7 +2426,7 @@
         <v>645002</v>
       </c>
       <c r="D46" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2427,7 +2440,7 @@
         <v>145057</v>
       </c>
       <c r="D47" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2511,7 +2524,7 @@
         <v>571200</v>
       </c>
       <c r="D53" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2525,7 +2538,7 @@
         <v>826045</v>
       </c>
       <c r="D54" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,7 +2650,7 @@
         <v>323283</v>
       </c>
       <c r="D62" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2707,7 +2720,7 @@
         <v>607756</v>
       </c>
       <c r="D67" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2749,7 +2762,7 @@
         <v>887998</v>
       </c>
       <c r="D70" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2860,7 @@
         <v>541447</v>
       </c>
       <c r="D77" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2889,7 +2902,7 @@
         <v>180705</v>
       </c>
       <c r="D80" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2903,7 +2916,7 @@
         <v>168099</v>
       </c>
       <c r="D81" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3071,7 +3084,7 @@
         <v>105809</v>
       </c>
       <c r="D93" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3099,7 +3112,7 @@
         <v>821702</v>
       </c>
       <c r="D95" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3113,7 +3126,7 @@
         <v>537590</v>
       </c>
       <c r="D96" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3127,7 +3140,7 @@
         <v>505469</v>
       </c>
       <c r="D97" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3197,7 +3210,7 @@
         <v>583538</v>
       </c>
       <c r="D102" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3211,7 +3224,7 @@
         <v>930683</v>
       </c>
       <c r="D103" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3295,7 +3308,7 @@
         <v>699260</v>
       </c>
       <c r="D109" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3309,7 +3322,7 @@
         <v>657791</v>
       </c>
       <c r="D110" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3323,7 +3336,7 @@
         <v>435653</v>
       </c>
       <c r="D111" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3337,7 +3350,7 @@
         <v>304624</v>
       </c>
       <c r="D112" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3365,7 +3378,7 @@
         <v>634090</v>
       </c>
       <c r="D114" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3435,7 +3448,7 @@
         <v>201963</v>
       </c>
       <c r="D119" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3463,7 +3476,7 @@
         <v>682553</v>
       </c>
       <c r="D121" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3547,7 +3560,7 @@
         <v>705184</v>
       </c>
       <c r="D127" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3659,7 +3672,7 @@
         <v>465368</v>
       </c>
       <c r="D135" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3701,7 +3714,7 @@
         <v>105601</v>
       </c>
       <c r="D138" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3715,7 +3728,7 @@
         <v>855773</v>
       </c>
       <c r="D139" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3743,7 +3756,7 @@
         <v>144447</v>
       </c>
       <c r="D141" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3771,7 +3784,7 @@
         <v>380335</v>
       </c>
       <c r="D143" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3785,7 +3798,7 @@
         <v>486594</v>
       </c>
       <c r="D144" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3841,7 +3854,7 @@
         <v>324318</v>
       </c>
       <c r="D148" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3911,7 +3924,7 @@
         <v>577643</v>
       </c>
       <c r="D153" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3925,7 +3938,7 @@
         <v>152375</v>
       </c>
       <c r="D154" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3953,7 +3966,7 @@
         <v>913794</v>
       </c>
       <c r="D156" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3967,7 +3980,7 @@
         <v>420598</v>
       </c>
       <c r="D157" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3981,7 +3994,7 @@
         <v>437968</v>
       </c>
       <c r="D158" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4023,7 +4036,7 @@
         <v>770758</v>
       </c>
       <c r="D161" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4079,7 +4092,7 @@
         <v>694075</v>
       </c>
       <c r="D165" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4093,7 +4106,7 @@
         <v>603297</v>
       </c>
       <c r="D166" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4121,7 +4134,7 @@
         <v>424250</v>
       </c>
       <c r="D168" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4135,7 +4148,7 @@
         <v>895417</v>
       </c>
       <c r="D169" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4191,7 +4204,7 @@
         <v>608250</v>
       </c>
       <c r="D173" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4303,7 +4316,7 @@
         <v>385261</v>
       </c>
       <c r="D181" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4345,7 +4358,7 @@
         <v>840851</v>
       </c>
       <c r="D184" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4443,7 +4456,7 @@
         <v>592280</v>
       </c>
       <c r="D191" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4485,7 +4498,7 @@
         <v>467124</v>
       </c>
       <c r="D194" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4513,7 +4526,7 @@
         <v>895693</v>
       </c>
       <c r="D196" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4541,7 +4554,7 @@
         <v>365239</v>
       </c>
       <c r="D198" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4653,7 +4666,7 @@
         <v>962384</v>
       </c>
       <c r="D206" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4723,7 +4736,7 @@
         <v>693918</v>
       </c>
       <c r="D211" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4737,7 +4750,7 @@
         <v>944148</v>
       </c>
       <c r="D212" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -4765,7 +4778,7 @@
         <v>653437</v>
       </c>
       <c r="D214" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4821,7 +4834,7 @@
         <v>879137</v>
       </c>
       <c r="D218" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4849,7 +4862,7 @@
         <v>713516</v>
       </c>
       <c r="D220" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4891,7 +4904,7 @@
         <v>925168</v>
       </c>
       <c r="D223" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4919,7 +4932,7 @@
         <v>932615</v>
       </c>
       <c r="D225" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4947,7 +4960,7 @@
         <v>762896</v>
       </c>
       <c r="D227" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4961,7 +4974,7 @@
         <v>807034</v>
       </c>
       <c r="D228" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4989,7 +5002,7 @@
         <v>129318</v>
       </c>
       <c r="D230" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5017,7 +5030,7 @@
         <v>940366</v>
       </c>
       <c r="D232" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5087,7 +5100,7 @@
         <v>988090</v>
       </c>
       <c r="D237" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5171,7 +5184,7 @@
         <v>804385</v>
       </c>
       <c r="D243" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5185,7 +5198,7 @@
         <v>745478</v>
       </c>
       <c r="D244" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5199,7 +5212,7 @@
         <v>985735</v>
       </c>
       <c r="D245" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5213,7 +5226,7 @@
         <v>499015</v>
       </c>
       <c r="D246" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5227,7 +5240,7 @@
         <v>235766</v>
       </c>
       <c r="D247" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5269,7 +5282,7 @@
         <v>865738</v>
       </c>
       <c r="D250" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -5283,7 +5296,7 @@
         <v>502948</v>
       </c>
       <c r="D251" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5395,7 +5408,7 @@
         <v>103682</v>
       </c>
       <c r="D259" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5479,7 +5492,7 @@
         <v>992440</v>
       </c>
       <c r="D265" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5507,7 +5520,7 @@
         <v>269490</v>
       </c>
       <c r="D267" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5521,7 +5534,7 @@
         <v>962921</v>
       </c>
       <c r="D268" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5605,7 +5618,7 @@
         <v>460614</v>
       </c>
       <c r="D274" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5619,7 +5632,7 @@
         <v>413737</v>
       </c>
       <c r="D275" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5633,7 +5646,7 @@
         <v>388326</v>
       </c>
       <c r="D276" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5647,7 +5660,7 @@
         <v>440377</v>
       </c>
       <c r="D277" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5661,7 +5674,7 @@
         <v>447117</v>
       </c>
       <c r="D278" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5675,7 +5688,7 @@
         <v>200081</v>
       </c>
       <c r="D279" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5689,7 +5702,7 @@
         <v>644185</v>
       </c>
       <c r="D280" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5703,7 +5716,7 @@
         <v>350504</v>
       </c>
       <c r="D281" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5717,7 +5730,7 @@
         <v>682826</v>
       </c>
       <c r="D282" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5731,7 +5744,7 @@
         <v>301774</v>
       </c>
       <c r="D283" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5745,7 +5758,7 @@
         <v>387943</v>
       </c>
       <c r="D284" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5773,7 +5786,7 @@
         <v>699016</v>
       </c>
       <c r="D286" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5787,7 +5800,7 @@
         <v>483197</v>
       </c>
       <c r="D287" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5801,7 +5814,7 @@
         <v>774263</v>
       </c>
       <c r="D288" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5815,7 +5828,7 @@
         <v>650738</v>
       </c>
       <c r="D289" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5857,7 +5870,7 @@
         <v>862581</v>
       </c>
       <c r="D292" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5885,7 +5898,7 @@
         <v>545433</v>
       </c>
       <c r="D294" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5913,7 +5926,7 @@
         <v>257041</v>
       </c>
       <c r="D296" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5941,7 +5954,7 @@
         <v>835085</v>
       </c>
       <c r="D298" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5997,7 +6010,7 @@
         <v>695453</v>
       </c>
       <c r="D302" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="303" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6011,7 +6024,7 @@
         <v>714712</v>
       </c>
       <c r="D303" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6025,7 +6038,7 @@
         <v>140374</v>
       </c>
       <c r="D304" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6081,7 +6094,7 @@
         <v>332941</v>
       </c>
       <c r="D308" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6095,7 +6108,7 @@
         <v>177963</v>
       </c>
       <c r="D309" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="310" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6109,7 +6122,7 @@
         <v>523692</v>
       </c>
       <c r="D310" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6123,7 +6136,7 @@
         <v>623505</v>
       </c>
       <c r="D311" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6137,7 +6150,7 @@
         <v>256948</v>
       </c>
       <c r="D312" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="313" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6165,7 +6178,7 @@
         <v>469032</v>
       </c>
       <c r="D314" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6179,7 +6192,7 @@
         <v>644342</v>
       </c>
       <c r="D315" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6193,7 +6206,7 @@
         <v>908581</v>
       </c>
       <c r="D316" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6207,7 +6220,7 @@
         <v>963896</v>
       </c>
       <c r="D317" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6221,7 +6234,7 @@
         <v>116706</v>
       </c>
       <c r="D318" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6249,7 +6262,7 @@
         <v>398667</v>
       </c>
       <c r="D320" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6263,7 +6276,7 @@
         <v>573879</v>
       </c>
       <c r="D321" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6277,7 +6290,7 @@
         <v>463574</v>
       </c>
       <c r="D322" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6291,7 +6304,7 @@
         <v>108261</v>
       </c>
       <c r="D323" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6305,7 +6318,7 @@
         <v>513946</v>
       </c>
       <c r="D324" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="325" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6319,7 +6332,7 @@
         <v>105016</v>
       </c>
       <c r="D325" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6347,7 +6360,7 @@
         <v>976807</v>
       </c>
       <c r="D327" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6375,7 +6388,7 @@
         <v>600517</v>
       </c>
       <c r="D329" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6417,7 +6430,7 @@
         <v>434100</v>
       </c>
       <c r="D332" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6445,7 +6458,7 @@
         <v>522482</v>
       </c>
       <c r="D334" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6473,7 +6486,7 @@
         <v>242285</v>
       </c>
       <c r="D336" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6529,7 +6542,7 @@
         <v>182736</v>
       </c>
       <c r="D340" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6543,7 +6556,7 @@
         <v>140919</v>
       </c>
       <c r="D341" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6557,7 +6570,7 @@
         <v>673265</v>
       </c>
       <c r="D342" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6571,7 +6584,7 @@
         <v>846610</v>
       </c>
       <c r="D343" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6585,7 +6598,7 @@
         <v>118022</v>
       </c>
       <c r="D344" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6599,7 +6612,7 @@
         <v>228377</v>
       </c>
       <c r="D345" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6627,7 +6640,7 @@
         <v>930583</v>
       </c>
       <c r="D347" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="348" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6655,7 +6668,7 @@
         <v>649727</v>
       </c>
       <c r="D349" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6669,7 +6682,7 @@
         <v>949478</v>
       </c>
       <c r="D350" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6697,7 +6710,7 @@
         <v>190844</v>
       </c>
       <c r="D352" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="353" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6711,7 +6724,7 @@
         <v>415462</v>
       </c>
       <c r="D353" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="354" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6767,7 +6780,7 @@
         <v>189348</v>
       </c>
       <c r="D357" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="358" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6823,7 +6836,7 @@
         <v>298538</v>
       </c>
       <c r="D361" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="362" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6837,7 +6850,7 @@
         <v>852722</v>
       </c>
       <c r="D362" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7019,7 +7032,7 @@
         <v>341061</v>
       </c>
       <c r="D375" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7075,7 +7088,7 @@
         <v>795061</v>
       </c>
       <c r="D379" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="380" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>